<commit_message>
cooling and ventilation logic added
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Scenario_HeatingTechnology_Availability.xlsx
+++ b/projects/test_building/input/Scenario_HeatingTechnology_Availability.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CA36A3-DC0B-3941-8CDF-4FE1A476B868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="6300" yWindow="4060" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6300" yWindow="4065" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -160,7 +159,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -216,53 +215,53 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:AR26" totalsRowShown="0">
-  <autoFilter ref="A1:AR26" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AR26" totalsRowShown="0">
+  <autoFilter ref="A1:AR26"/>
   <tableColumns count="44">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="id_region"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="id_heating_technology"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="unit"/>
-    <tableColumn id="35" xr3:uid="{D983A755-D09D-2549-B077-D834C9C968AB}" name="2010"/>
-    <tableColumn id="36" xr3:uid="{EB98B56D-FE23-DF42-836E-7071CF499087}" name="2011"/>
-    <tableColumn id="37" xr3:uid="{32766B77-AA94-1748-988B-E5F51B823EFB}" name="2012"/>
-    <tableColumn id="38" xr3:uid="{EF9FABBD-5E33-5F4A-A9CF-CC5F0B34E1FB}" name="2013"/>
-    <tableColumn id="39" xr3:uid="{D5858403-3CB0-494F-BD32-96DF39AD7186}" name="2014"/>
-    <tableColumn id="40" xr3:uid="{C0CC9032-5BC5-A14B-BEB6-6C215571E4BA}" name="2015"/>
-    <tableColumn id="41" xr3:uid="{223293F8-97B3-EF48-AB8F-EB1053FF5A06}" name="2016"/>
-    <tableColumn id="42" xr3:uid="{56743070-278C-BE45-A140-82A50FEE3012}" name="2017"/>
-    <tableColumn id="43" xr3:uid="{EC984FBB-E428-EF45-98C9-04A1820BB3D3}" name="2018"/>
-    <tableColumn id="44" xr3:uid="{F5CE8AE9-4B9B-6549-887A-0B7F8FF877C4}" name="2019"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="2020"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="2021"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="2022"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="2023"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="2024"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="2025"/>
-    <tableColumn id="45" xr3:uid="{A7D13675-55B4-E546-9D38-D874D2349974}" name="2026"/>
-    <tableColumn id="46" xr3:uid="{E126CBA9-F862-4849-8F96-DA247B05B9B2}" name="2027"/>
-    <tableColumn id="47" xr3:uid="{B5892AA7-A4A2-AD49-A294-0718CF4092EC}" name="2028"/>
-    <tableColumn id="48" xr3:uid="{5F8C2E0B-B34A-2D41-BE22-98777CBCAA5B}" name="2029"/>
-    <tableColumn id="49" xr3:uid="{C794D40D-4398-1B41-988A-50F7B7CDAC2B}" name="2030"/>
-    <tableColumn id="50" xr3:uid="{4FDFD7CF-E070-974B-9871-ABB63D6BD90E}" name="2031"/>
-    <tableColumn id="51" xr3:uid="{52157ADD-7961-8A40-869C-9F7467134DAE}" name="2032"/>
-    <tableColumn id="52" xr3:uid="{9F60C393-A13B-DB45-925B-8771FC49C310}" name="2033"/>
-    <tableColumn id="53" xr3:uid="{C152417E-23A9-6946-BEAA-A149CE766058}" name="2034"/>
-    <tableColumn id="54" xr3:uid="{867E06D4-D62D-6841-80A8-C409FC424508}" name="2035"/>
-    <tableColumn id="55" xr3:uid="{D5F8013B-3B2C-6041-B5EF-BB27BB484B2F}" name="2036"/>
-    <tableColumn id="56" xr3:uid="{1352DC67-B667-F741-88CD-053192ED6EF1}" name="2037"/>
-    <tableColumn id="57" xr3:uid="{CF4FF0F5-7B49-734E-8F84-45C2DFD50341}" name="2038"/>
-    <tableColumn id="58" xr3:uid="{0741A53F-B1B9-4C4B-9227-99A936AC9857}" name="2039"/>
-    <tableColumn id="59" xr3:uid="{B6539615-6EA3-E84B-A8BD-3BFADF9DFCE0}" name="2040"/>
-    <tableColumn id="60" xr3:uid="{6EF55F9B-4377-F743-B699-991A17B31F9F}" name="2041"/>
-    <tableColumn id="61" xr3:uid="{E7420824-86F0-3147-A918-F2DCAD872C13}" name="2042"/>
-    <tableColumn id="62" xr3:uid="{FAED8714-1A7C-5646-A387-35236ED4F657}" name="2043"/>
-    <tableColumn id="63" xr3:uid="{0568332B-9040-684F-8C4A-73A7CF2F8AAA}" name="2044"/>
-    <tableColumn id="64" xr3:uid="{6FACD85D-EAC7-6D4E-B761-BA89E6B51753}" name="2045"/>
-    <tableColumn id="65" xr3:uid="{67B57015-A858-5145-B258-B9C2EBEB664C}" name="2046"/>
-    <tableColumn id="66" xr3:uid="{0214A31B-DB0B-0342-888B-797534C66924}" name="2047"/>
-    <tableColumn id="67" xr3:uid="{68422419-527A-AC49-BFB7-DE62A7EB15FD}" name="2048"/>
-    <tableColumn id="68" xr3:uid="{1760A3CF-AC68-CC4D-85C1-3BBE51BCF94F}" name="2049"/>
-    <tableColumn id="69" xr3:uid="{947A96E4-9491-AD4F-BFD0-8DB3EA4D22D3}" name="2050"/>
+    <tableColumn id="2" name="id_region"/>
+    <tableColumn id="3" name="id_heating_technology"/>
+    <tableColumn id="4" name="unit"/>
+    <tableColumn id="35" name="2010"/>
+    <tableColumn id="36" name="2011"/>
+    <tableColumn id="37" name="2012"/>
+    <tableColumn id="38" name="2013"/>
+    <tableColumn id="39" name="2014"/>
+    <tableColumn id="40" name="2015"/>
+    <tableColumn id="41" name="2016"/>
+    <tableColumn id="42" name="2017"/>
+    <tableColumn id="43" name="2018"/>
+    <tableColumn id="44" name="2019"/>
+    <tableColumn id="5" name="2020"/>
+    <tableColumn id="6" name="2021"/>
+    <tableColumn id="7" name="2022"/>
+    <tableColumn id="8" name="2023"/>
+    <tableColumn id="9" name="2024"/>
+    <tableColumn id="10" name="2025"/>
+    <tableColumn id="45" name="2026"/>
+    <tableColumn id="46" name="2027"/>
+    <tableColumn id="47" name="2028"/>
+    <tableColumn id="48" name="2029"/>
+    <tableColumn id="49" name="2030"/>
+    <tableColumn id="50" name="2031"/>
+    <tableColumn id="51" name="2032"/>
+    <tableColumn id="52" name="2033"/>
+    <tableColumn id="53" name="2034"/>
+    <tableColumn id="54" name="2035"/>
+    <tableColumn id="55" name="2036"/>
+    <tableColumn id="56" name="2037"/>
+    <tableColumn id="57" name="2038"/>
+    <tableColumn id="58" name="2039"/>
+    <tableColumn id="59" name="2040"/>
+    <tableColumn id="60" name="2041"/>
+    <tableColumn id="61" name="2042"/>
+    <tableColumn id="62" name="2043"/>
+    <tableColumn id="63" name="2044"/>
+    <tableColumn id="64" name="2045"/>
+    <tableColumn id="65" name="2046"/>
+    <tableColumn id="66" name="2047"/>
+    <tableColumn id="67" name="2048"/>
+    <tableColumn id="68" name="2049"/>
+    <tableColumn id="69" name="2050"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -530,22 +529,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="13" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -679,7 +678,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>9</v>
       </c>
@@ -813,7 +812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>9</v>
       </c>
@@ -947,7 +946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>9</v>
       </c>
@@ -1081,7 +1080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9</v>
       </c>
@@ -1215,7 +1214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>9</v>
       </c>
@@ -1349,7 +1348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>9</v>
       </c>
@@ -1483,7 +1482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9</v>
       </c>
@@ -1617,7 +1616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -1751,7 +1750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1885,7 +1884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2019,7 +2018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -2153,7 +2152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -2287,7 +2286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>9</v>
       </c>
@@ -2421,7 +2420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>9</v>
       </c>
@@ -2555,7 +2554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>9</v>
       </c>
@@ -2689,7 +2688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>9</v>
       </c>
@@ -2823,7 +2822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>9</v>
       </c>
@@ -2957,7 +2956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>9</v>
       </c>
@@ -3091,7 +3090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>9</v>
       </c>
@@ -3225,7 +3224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>9</v>
       </c>
@@ -3359,7 +3358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>9</v>
       </c>
@@ -3493,7 +3492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>9</v>
       </c>
@@ -3627,7 +3626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>9</v>
       </c>
@@ -3761,7 +3760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>9</v>
       </c>
@@ -3895,7 +3894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
update of infrastructure and heating technology availability for historic and future scenario simulations
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Scenario_HeatingTechnology_Availability.xlsx
+++ b/projects/test_building/input/Scenario_HeatingTechnology_Availability.xlsx
@@ -537,7 +537,7 @@
   <dimension ref="A1:AS76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG87" sqref="AG87"/>
+      <selection activeCell="J32" sqref="J32:N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4825,19 +4825,19 @@
         <v>1</v>
       </c>
       <c r="J32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O32">
         <v>0</v>

</xml_diff>